<commit_message>
Adding CLX class to binary encoded substance usage variables
</commit_message>
<xml_diff>
--- a/Usage_Variables_Binary_Example.xlsx
+++ b/Usage_Variables_Binary_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bateu\OneDrive\Masters\STAT5003\Assignment\GitHub_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CEFA1C-B21C-44C9-9851-2024F7AC62A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D30874D-A97C-402A-8543-4A08A6157FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="34560" windowHeight="18684" xr2:uid="{80773B18-662D-4EEC-9EF4-41C33CD133A2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{80773B18-662D-4EEC-9EF4-41C33CD133A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Chris Bateup</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{EF27ABD8-2E9D-434A-AAB4-FCCCAA6EB060}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Bateup:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+We've added an additional level which is effectively, used less than 99 years ago.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>CL0</t>
   </si>
@@ -72,9 +106,6 @@
   </si>
   <si>
     <t>ly_1d</t>
-  </si>
-  <si>
-    <t>usage</t>
   </si>
   <si>
     <t>usage_numeric</t>
@@ -133,38 +164,50 @@
     </r>
   </si>
   <si>
-    <t>vsa_numeric</t>
-  </si>
-  <si>
-    <t>vsa_CL0</t>
-  </si>
-  <si>
-    <t>vsa_CL1</t>
-  </si>
-  <si>
-    <t>vsa_CL2</t>
-  </si>
-  <si>
-    <t>vsa_CL3</t>
-  </si>
-  <si>
-    <t>vsa_CL4</t>
-  </si>
-  <si>
-    <t>vsa_CL5</t>
-  </si>
-  <si>
-    <t>vsa_CL6</t>
-  </si>
-  <si>
     <t>Extract from data:</t>
+  </si>
+  <si>
+    <t>lt99y</t>
+  </si>
+  <si>
+    <t>CLX</t>
+  </si>
+  <si>
+    <t>alcohol_CL0</t>
+  </si>
+  <si>
+    <t>alcohol_CL1</t>
+  </si>
+  <si>
+    <t>alcohol_CLX</t>
+  </si>
+  <si>
+    <t>alcohol_CL2</t>
+  </si>
+  <si>
+    <t>alcohol_CL3</t>
+  </si>
+  <si>
+    <t>alcohol_CL4</t>
+  </si>
+  <si>
+    <t>alcohol_CL5</t>
+  </si>
+  <si>
+    <t>alcohol_CL6</t>
+  </si>
+  <si>
+    <t>alcohol_numeric</t>
+  </si>
+  <si>
+    <t>original_usage_variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,26 +247,52 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="7"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4E5C68"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -280,11 +349,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -309,12 +398,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,27 +729,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2363A36-1F48-4C83-97D8-EC12348D01DF}">
-  <dimension ref="A1:Y30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2363A36-1F48-4C83-97D8-EC12348D01DF}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="23" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="24" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
@@ -657,396 +757,428 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>"CL"&amp;B4</f>
+        <f t="shared" ref="A4:A10" si="0">"CL"&amp;B4</f>
         <v>CL0</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="8">
-        <f>IF($B4&lt;&gt;C$2,0,1)</f>
+        <f t="shared" ref="C4:D10" si="1">IF($B4&lt;&gt;C$2,0,1)</f>
         <v>1</v>
       </c>
       <c r="D4" s="9">
-        <f>IF($B4&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <f>IF($B4&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="17">
         <v>0</v>
       </c>
       <c r="F4" s="10">
-        <f>IF($B4&lt;F$2,0,1)</f>
+        <f t="shared" ref="F4:J10" si="2">IF($B4&lt;F$2,0,1)</f>
         <v>0</v>
       </c>
       <c r="G4" s="10">
-        <f>IF($B4&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H4" s="10">
-        <f>IF($B4&lt;H$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <f>IF($B4&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>"CL"&amp;B5</f>
+        <f t="shared" si="0"/>
         <v>CL1</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="8">
-        <f>IF($B5&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D5" s="9">
-        <f>IF($B5&lt;&gt;D$2,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
-        <f>IF($B5&lt;E$2,0,1)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
       </c>
       <c r="F5" s="10">
-        <f>IF($B5&lt;F$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G5" s="10">
-        <f>IF($B5&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="10">
-        <f>IF($B5&lt;H$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="9">
-        <f>IF($B5&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>"CL"&amp;B6</f>
+        <f t="shared" si="0"/>
         <v>CL2</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="8">
-        <f>IF($B6&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6" s="9">
-        <f>IF($B6&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <f>IF($B6&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
         <v>1</v>
       </c>
       <c r="F6" s="10">
-        <f>IF($B6&lt;F$2,0,1)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="G6" s="10">
-        <f>IF($B6&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H6" s="10">
-        <f>IF($B6&lt;H$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <f>IF($B6&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>"CL"&amp;B7</f>
+        <f t="shared" si="0"/>
         <v>CL3</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" s="8">
-        <f>IF($B7&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D7" s="9">
-        <f>IF($B7&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
-        <f>IF($B7&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
         <v>1</v>
       </c>
       <c r="F7" s="10">
-        <f>IF($B7&lt;F$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G7" s="10">
-        <f>IF($B7&lt;G$2,0,1)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="H7" s="10">
-        <f>IF($B7&lt;H$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <f>IF($B7&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>"CL"&amp;B8</f>
+        <f t="shared" si="0"/>
         <v>CL4</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" s="8">
-        <f>IF($B8&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D8" s="9">
-        <f>IF($B8&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <f>IF($B8&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
         <v>1</v>
       </c>
       <c r="F8" s="10">
-        <f>IF($B8&lt;F$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G8" s="10">
-        <f>IF($B8&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8" s="10">
-        <f>IF($B8&lt;H$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <f>IF($B8&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>"CL"&amp;B9</f>
+        <f t="shared" si="0"/>
         <v>CL5</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" s="8">
-        <f>IF($B9&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9" s="9">
-        <f>IF($B9&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
-        <f>IF($B9&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
         <v>1</v>
       </c>
       <c r="F9" s="10">
-        <f>IF($B9&lt;F$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9" s="10">
-        <f>IF($B9&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H9" s="10">
-        <f>IF($B9&lt;H$2,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="9">
-        <f>IF($B9&lt;I$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>"CL"&amp;B10</f>
+        <f t="shared" si="0"/>
         <v>CL6</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" s="8">
-        <f>IF($B10&lt;&gt;C$2,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10" s="9">
-        <f>IF($B10&lt;&gt;D$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <f>IF($B10&lt;E$2,0,1)</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
         <v>1</v>
       </c>
       <c r="F10" s="10">
-        <f>IF($B10&lt;F$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G10" s="10">
-        <f>IF($B10&lt;G$2,0,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H10" s="10">
-        <f>IF($B10&lt;H$2,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="9">
-        <f>IF($B10&lt;I$2,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="13"/>
+      <c r="C13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="14">
-        <v>0</v>
+      <c r="K13" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="12">
+        <v>1</v>
       </c>
       <c r="C14" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="14">
         <v>0</v>
@@ -1063,22 +1195,28 @@
       <c r="I14" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
-        <v>1</v>
+      <c r="J14" s="14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="12">
+        <v>2</v>
       </c>
       <c r="C15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="14">
         <v>0</v>
@@ -1089,26 +1227,31 @@
       <c r="I15" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14">
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="12">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14">
         <v>2</v>
       </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
       <c r="D16" s="14">
         <v>0</v>
       </c>
       <c r="E16" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="14">
         <v>0</v>
@@ -1116,48 +1259,57 @@
       <c r="I16" s="14">
         <v>0</v>
       </c>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14">
+      <c r="J16" s="14">
+        <v>0</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="12">
+        <v>4</v>
+      </c>
+      <c r="C17" s="14">
         <v>3</v>
       </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
       <c r="D17" s="14">
         <v>0</v>
       </c>
       <c r="E17" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="14">
         <v>1</v>
       </c>
       <c r="G17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="14">
         <v>0</v>
       </c>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B18" s="14">
+      <c r="J17" s="14">
+        <v>0</v>
+      </c>
+      <c r="K17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="12">
+        <v>5</v>
+      </c>
+      <c r="C18" s="14">
         <v>4</v>
       </c>
-      <c r="C18" s="14">
-        <v>0</v>
-      </c>
       <c r="D18" s="14">
         <v>0</v>
       </c>
       <c r="E18" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="14">
         <v>1</v>
@@ -1166,25 +1318,30 @@
         <v>1</v>
       </c>
       <c r="H18" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="14">
-        <v>0</v>
-      </c>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B19" s="14">
+        <v>1</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="12">
+        <v>6</v>
+      </c>
+      <c r="C19" s="14">
         <v>5</v>
       </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
       <c r="D19" s="14">
         <v>0</v>
       </c>
       <c r="E19" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="14">
         <v>1</v>
@@ -1196,22 +1353,27 @@
         <v>1</v>
       </c>
       <c r="I19" s="14">
-        <v>0</v>
-      </c>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="14">
+        <v>1</v>
+      </c>
+      <c r="J19" s="14">
+        <v>1</v>
+      </c>
+      <c r="K19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="12">
+        <v>7</v>
+      </c>
+      <c r="C20" s="14">
         <v>6</v>
       </c>
-      <c r="C20" s="14">
-        <v>0</v>
-      </c>
       <c r="D20" s="14">
         <v>0</v>
       </c>
       <c r="E20" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="14">
         <v>1</v>
@@ -1225,93 +1387,17 @@
       <c r="I20" s="14">
         <v>1</v>
       </c>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
-      <c r="U30" s="12"/>
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="12"/>
-      <c r="Y30" s="12"/>
+      <c r="J20" s="14">
+        <v>1</v>
+      </c>
+      <c r="K20" s="14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>